<commit_message>
Simplify scores to make visual comparison easier
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -166,13 +166,15 @@
   </sheetPr>
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81:B101"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,7 +190,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>350199</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,7 +198,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>222060</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -204,7 +206,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>4288</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -212,7 +214,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>558481</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -220,7 +222,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>419597</v>
+        <v>597</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,7 +230,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>499410</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,7 +238,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>243880</v>
+        <v>880</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +246,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>363427</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,7 +254,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>524828</v>
+        <v>828</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,7 +262,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>519391</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,7 +270,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>728330</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,7 +278,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>409399</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +286,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>814989</v>
+        <v>989</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,7 +294,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>981280</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,7 +302,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>946633</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,7 +310,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>900807</v>
+        <v>807</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +318,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>564439</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +326,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>508758</v>
+        <v>758</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +334,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>763003</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +342,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>329607</v>
+        <v>607</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,7 +350,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>905376</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +358,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>557674</v>
+        <v>674</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +366,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>365261</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>203375</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +382,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>313933</v>
+        <v>933</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +390,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>695527</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,7 +398,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>5030</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>418214</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,7 +414,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>134482</v>
+        <v>482</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,7 +422,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>688907</v>
+        <v>907</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>604543</v>
+        <v>543</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>890064</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>591222</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +454,7 @@
         <v>10</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>498903</v>
+        <v>903</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +462,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>807734</v>
+        <v>734</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>723043</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +478,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>543445</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>509530</v>
+        <v>530</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,7 +494,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>544169</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>329446</v>
+        <v>446</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>695649</v>
+        <v>649</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>70770</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>195482</v>
+        <v>482</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>534595</v>
+        <v>595</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>522233</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,7 +550,7 @@
         <v>6</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>297721</v>
+        <v>721</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>401917</v>
+        <v>917</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>197694</v>
+        <v>694</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,7 +574,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>882269</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>754037</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>468555</v>
+        <v>555</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>557966</v>
+        <v>966</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>548839</v>
+        <v>839</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +614,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>156481</v>
+        <v>481</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>554908</v>
+        <v>908</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>87906</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>251749</v>
+        <v>749</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>355473</v>
+        <v>473</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>49331</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>796686</v>
+        <v>686</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>75870</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>76623</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>293798</v>
+        <v>798</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>136974</v>
+        <v>974</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>221598</v>
+        <v>598</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>326948</v>
+        <v>948</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>106516</v>
+        <v>516</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>513418</v>
+        <v>418</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>735284</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>867983</v>
+        <v>983</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>1330</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>241961</v>
+        <v>961</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>962882</v>
+        <v>882</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>224666</v>
+        <v>666</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>34644</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,7 +790,7 @@
         <v>5</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>850064</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>8385</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +806,7 @@
         <v>8</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>661464</v>
+        <v>464</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="2" t="n">
-        <v>665825</v>
+        <v>825</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>